<commit_message>
replace pattern per value 407ccc94deca8c9bcdd1a0762e7b646258f35c38
</commit_message>
<xml_diff>
--- a/nr-prepare-release-1.1.0/ig/StructureDefinition-as-device.xlsx
+++ b/nr-prepare-release-1.1.0/ig/StructureDefinition-as-device.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-11-13T10:02:18+00:00</t>
+    <t>2024-11-13T13:22:24+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -670,11 +670,11 @@
     <t>The barcode string from a barcode present on a device label or package may identify the instance, include names given to the device in local usage, or may identify the type of device. If the identifier identifies the type of device, Device.type element should be used.</t>
   </si>
   <si>
-    <t xml:space="preserve">pattern:system}
+    <t xml:space="preserve">value:system}
 </t>
   </si>
   <si>
-    <t>Slice based on the identifier.system pattern</t>
+    <t>Slice based on the identifier.system value</t>
   </si>
   <si>
     <t>.id</t>

</xml_diff>